<commit_message>
Adding SQL connection and project plan
</commit_message>
<xml_diff>
--- a/Project Plan/HR_Project_Schedule.xlsx
+++ b/Project Plan/HR_Project_Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaNdE\HR_Analysis\Project Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c8f1aedf5a35ac5/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34D2280-CA9D-4DB2-B054-0105DB183089}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="432" documentId="8_{BD233116-A664-48E5-A8A5-2DDCF96F0438}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00F83E77-CFB6-41BF-902A-203086407F2E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{02F4FD01-0C73-40F9-AD5F-74B5D3B2FC29}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <author>tc={290BB73A-EF1D-4E13-A19B-72DD54C9761C}</author>
   </authors>
   <commentList>
-    <comment ref="A12" authorId="0" shapeId="0" xr:uid="{290BB73A-EF1D-4E13-A19B-72DD54C9761C}">
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{290BB73A-EF1D-4E13-A19B-72DD54C9761C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
   <si>
     <t>Task Name</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Name our variables from the dataset and update variables in the code</t>
   </si>
   <si>
-    <t>Code the index file to include the div's from our dashboard design (TBD)</t>
-  </si>
-  <si>
     <t>Team Role Sign Up</t>
   </si>
   <si>
@@ -141,9 +138,6 @@
     <t>How does salary effect job satisfaction?</t>
   </si>
   <si>
-    <t>How does salary effect employee performance rating?</t>
-  </si>
-  <si>
     <t>Meter/Needle</t>
   </si>
   <si>
@@ -267,22 +261,106 @@
     <t>General Idea: Tie a monetary value to our proposed solutions--ie. Return on Investment (ROI) such as "pay a higher salary now for X employee but over 15 years save Y in training/education funding". This could add a financial analysis to the project and our own portfolios.</t>
   </si>
   <si>
-    <t>Find the top-indicators of a top peforming employee through exposing which variables in our dataset hold the strongest correlation.</t>
-  </si>
-  <si>
-    <t>Business Solution 1: Build a product we would hypothetically give to recruiters enabling them to "drag and drop in" submitted resumes that would search for these indicators and return the top 5 or so matching the specified criteria. We could build the front end using Javascript and use JSON on the backend to filter through the text in resumes.</t>
-  </si>
-  <si>
-    <t>Scope</t>
-  </si>
-  <si>
     <t>Sam</t>
   </si>
   <si>
+    <t>Proposal/Scope</t>
+  </si>
+  <si>
+    <t>Find a second data set to use for mapping</t>
+  </si>
+  <si>
     <t>All</t>
   </si>
   <si>
-    <t>Find second dataset for mapping</t>
+    <t>Code the index file to include the div's from our dashboard design</t>
+  </si>
+  <si>
+    <t>What factors hold the strongest correlation to our top performers?</t>
+  </si>
+  <si>
+    <t>Business Solution 1: Use this info to create a "product" we would hypothetically deliver to the Recruiting team, that could automate filtering through resumes with a "drag and drop" feature into a form we create with javascript and possibly through using JSON, to pull the resumes first that hold the characteristics we find are consistent among top performers in our company.</t>
+  </si>
+  <si>
+    <t>Machine Learning Engineer</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Project 3</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>How does marital status affect job satisfaction?</t>
+  </si>
+  <si>
+    <t>What was the performance category of employees who left the company?</t>
+  </si>
+  <si>
+    <t>How is job satisfaction affected by commuting distance?</t>
+  </si>
+  <si>
+    <t>How is job satisfaction affected by business travel?</t>
+  </si>
+  <si>
+    <t>How is job satisfaction affected by overtime?</t>
+  </si>
+  <si>
+    <t>How is job satisfaction affected by job role?</t>
+  </si>
+  <si>
+    <t>How does the education level affect the monthly rate/salary?</t>
+  </si>
+  <si>
+    <t>How does the department affect the monthly rate/salary?</t>
+  </si>
+  <si>
+    <t>How does gender affect salary overall in the company?</t>
+  </si>
+  <si>
+    <t>How does gender affect salary in each department of the company?</t>
+  </si>
+  <si>
+    <t>How does gender affect job satisfaction within each department?</t>
+  </si>
+  <si>
+    <t>How does your years in current role affect your job satisfaction?</t>
+  </si>
+  <si>
+    <t>How does your years since last promotion affect job satisfaction?</t>
+  </si>
+  <si>
+    <t>How does your years at the company affect your job satisfaction?</t>
+  </si>
+  <si>
+    <t>Average age of the employees</t>
+  </si>
+  <si>
+    <t>How does your age affect job satisfaction?</t>
+  </si>
+  <si>
+    <t>How does your department affect your job satisfaction?</t>
+  </si>
+  <si>
+    <t>How does last salary hike affect performance rating?</t>
+  </si>
+  <si>
+    <t>How does last salary hike affect job satisfaction?</t>
+  </si>
+  <si>
+    <t>How does performance rating affect salary?</t>
+  </si>
+  <si>
+    <t>Read dataset into group AWS</t>
+  </si>
+  <si>
+    <t>Read dataset into MySQL Workbench</t>
+  </si>
+  <si>
+    <t>Sandra</t>
   </si>
 </sst>
 </file>
@@ -380,7 +458,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -403,13 +481,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -420,12 +545,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -479,7 +602,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,15 +612,40 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,79 +715,6 @@
         <a:lstStyle/>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="3225800" cy="781240"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{980C6106-29F5-473D-BD95-B7ED46B77868}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9017000" y="831850"/>
-          <a:ext cx="3225800" cy="781240"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln>
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Data</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
-            <a:t> analysis questions are above the gray line, whereas some data we could showcase as sort of an "overview of where we are" is below the gray line. Just some ideas :)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -952,7 +1026,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A12" dT="2021-02-02T22:44:04.67" personId="{980333BF-B200-4403-B1E3-1C6C58F93070}" id="{290BB73A-EF1D-4E13-A19B-72DD54C9761C}">
+  <threadedComment ref="A14" dT="2021-02-02T22:44:04.67" personId="{980333BF-B200-4403-B1E3-1C6C58F93070}" id="{290BB73A-EF1D-4E13-A19B-72DD54C9761C}">
     <text>The instructions for the step are available at https://zoom.us/rec/play/Qw04fYFMUsRIXLak1TvswfIDqmPwoV16FvN4WGobshjUTySXNjvFWznQNB5b5pZgs6qRZCUK2SbFpBXi.yUvOevLRk7398GsV ... 4:33 in the video</text>
   </threadedComment>
 </ThreadedComments>
@@ -960,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401E91F5-96CF-4A59-947D-268E9EC6FF85}">
-  <dimension ref="A1:P25"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -971,412 +1045,421 @@
     <col min="1" max="1" width="69.7265625" customWidth="1"/>
     <col min="2" max="2" width="17.36328125" customWidth="1"/>
     <col min="3" max="3" width="26.54296875" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.1796875" style="44" customWidth="1"/>
+    <col min="5" max="5" width="32" style="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.4">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="34"/>
-      <c r="L1" s="34"/>
-      <c r="M1" s="34"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-    </row>
-    <row r="2" spans="1:16" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" s="31">
-        <f>E2-D2</f>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+    </row>
+    <row r="2" spans="1:16" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="28">
         <v>0</v>
       </c>
-      <c r="D2" s="32">
+      <c r="D2" s="29">
         <v>44228</v>
       </c>
-      <c r="E2" s="32">
+      <c r="E2" s="29">
         <v>44228</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-    </row>
-    <row r="3" spans="1:16" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A3" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="31">
-        <f t="shared" ref="C3:C25" si="0">E3-D3</f>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+    </row>
+    <row r="3" spans="1:16" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="28">
+        <f>E3-D3</f>
         <v>2</v>
       </c>
-      <c r="D3" s="32">
+      <c r="D3" s="29">
         <v>44229</v>
       </c>
-      <c r="E3" s="32">
+      <c r="E3" s="29">
         <v>44231</v>
       </c>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-    </row>
-    <row r="4" spans="1:16" s="8" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A4" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="31">
-        <f t="shared" si="0"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+    </row>
+    <row r="4" spans="1:16" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="28">
+        <f>E4-D4</f>
         <v>2</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="29">
         <v>44229</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="29">
         <v>44231</v>
       </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31">
+      <c r="A5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="28">
+        <f t="shared" ref="C5:C12" si="0">E5-D5</f>
+        <v>0</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="28">
+        <f>E6-D6</f>
+        <v>0</v>
+      </c>
+      <c r="D6" s="43">
+        <v>44231</v>
+      </c>
+      <c r="E6" s="43">
+        <v>44231</v>
+      </c>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="31"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="31"/>
+      <c r="P6" s="31"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-      <c r="P5" s="35"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="31">
+      <c r="D7" s="43">
+        <v>44231</v>
+      </c>
+      <c r="E7" s="43">
+        <v>44231</v>
+      </c>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31"/>
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
-      <c r="P6" s="35"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="31">
+      <c r="D8" s="43">
+        <v>44231</v>
+      </c>
+      <c r="E8" s="43">
+        <v>44231</v>
+      </c>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35"/>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="12" t="s">
+      <c r="D9" s="43">
+        <v>44231</v>
+      </c>
+      <c r="E9" s="43">
+        <v>44231</v>
+      </c>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="31">
+      <c r="B10" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35"/>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-      <c r="H10" s="35"/>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="35"/>
-      <c r="M10" s="35"/>
-      <c r="N10" s="35"/>
-      <c r="O10" s="35"/>
-      <c r="P10" s="35"/>
+      <c r="D10" s="43">
+        <v>44231</v>
+      </c>
+      <c r="E10" s="43">
+        <v>44231</v>
+      </c>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="35"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-      <c r="N11" s="35"/>
-      <c r="O11" s="35"/>
-      <c r="P11" s="35"/>
+      <c r="A11" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
+      <c r="L11" s="31"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
+      <c r="P11" s="31"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="35"/>
-      <c r="P12" s="35"/>
+      <c r="A12" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="43">
+        <v>44231</v>
+      </c>
+      <c r="E12" s="43"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C13" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C14" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="A14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="C15" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="A15" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C21" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C23" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C25" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1396,14 +1479,17 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="E2" sqref="E2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="7" max="7" width="26.08984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -1415,128 +1501,170 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="36"/>
       <c r="C2" s="36"/>
       <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="E2" s="36" t="s">
+        <v>16</v>
+      </c>
       <c r="F2" s="36"/>
       <c r="G2" s="36"/>
       <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
       <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="E3" s="36" t="s">
+        <v>20</v>
+      </c>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="36"/>
       <c r="C4" s="36"/>
       <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="E4" s="36" t="s">
+        <v>17</v>
+      </c>
       <c r="F4" s="36"/>
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="36" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
       <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36"/>
+      <c r="E5" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="41"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="36" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="36"/>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
+      <c r="E6" s="36" t="s">
+        <v>15</v>
+      </c>
       <c r="F6" s="36"/>
       <c r="G6" s="36"/>
       <c r="H6" s="36"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C9" s="37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
+      <c r="G9" s="33" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C10" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="36"/>
       <c r="E10" s="36"/>
       <c r="F10" s="36"/>
+      <c r="G10" s="32" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C11" s="36" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" s="36"/>
       <c r="E11" s="36"/>
       <c r="F11" s="36"/>
+      <c r="G11" s="32" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C12" s="36" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="36"/>
       <c r="E12" s="36"/>
       <c r="F12" s="36"/>
+      <c r="G12" s="32" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C13" s="36" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="36"/>
       <c r="E13" s="36"/>
       <c r="F13" s="36"/>
+      <c r="G13" s="32" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C14" s="36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
+      <c r="G14" s="32" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C15" s="36" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="36"/>
       <c r="E15" s="36"/>
       <c r="F15" s="36"/>
+      <c r="G15" s="32" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
+      <c r="C16" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="32" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
+  <mergeCells count="19">
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:D2"/>
@@ -1550,188 +1678,317 @@
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A106429C-D134-43D9-BF1B-C443895E320D}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="61.81640625" customWidth="1"/>
-    <col min="2" max="2" width="42.90625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="16" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="17" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="14"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="17"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="14"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="17"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="17" t="s">
+      <c r="B4" s="18"/>
+      <c r="C4" s="14"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="17"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="17" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="14"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="14"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="18"/>
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="18"/>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="18"/>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="18"/>
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="18"/>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="18"/>
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="18"/>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="18"/>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="18"/>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="45" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="18"/>
+      <c r="C17" s="14"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="18"/>
+      <c r="C18" s="14"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="18"/>
+      <c r="C19" s="14"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="18"/>
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="14"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="14"/>
+    </row>
+    <row r="25" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="17"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="17"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="17"/>
-    </row>
-    <row r="7" spans="1:3" ht="5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="20"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="20"/>
-    </row>
-    <row r="8" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="17" t="s">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="14"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="21"/>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="17" t="s">
+      <c r="B30" s="18"/>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="21"/>
-      <c r="C10" s="17"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="17" t="s">
+      <c r="B31" s="18"/>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="17"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="17" t="s">
+      <c r="B32" s="18"/>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="21"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="17" t="s">
+      <c r="B33" s="18"/>
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="17"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="17" t="s">
+      <c r="B34" s="18"/>
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="21"/>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
+      <c r="B35" s="18"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="21"/>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="17" t="s">
+      <c r="B36" s="18"/>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="21"/>
-      <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="17" t="s">
+      <c r="B37" s="18"/>
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="17"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="17" t="s">
+      <c r="B38" s="18"/>
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="21"/>
-      <c r="C18" s="17"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="17"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="17"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="17"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="19"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="14"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="18"/>
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="16"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1745,7 +2002,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1754,78 +2011,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="22"/>
+    </row>
+    <row r="2" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
+      <c r="B3" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="4"/>
+      <c r="B4" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="25"/>
-    </row>
-    <row r="2" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="28" t="s">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="4">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="28" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
-        <v>2</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>65</v>
-      </c>
-    </row>
     <row r="6" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="29" t="s">
-        <v>69</v>
+      <c r="B6" s="26" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="39">
+      <c r="A7" s="34">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>70</v>
+      <c r="B7" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="7"/>
-      <c r="B8" s="40" t="s">
-        <v>71</v>
+      <c r="A8" s="5"/>
+      <c r="B8" s="35" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding updated web template and supporting files
</commit_message>
<xml_diff>
--- a/Project Plan/HR_Project_Schedule.xlsx
+++ b/Project Plan/HR_Project_Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6c8f1aedf5a35ac5/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaNdE\HR_Analysis\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="432" documentId="8_{BD233116-A664-48E5-A8A5-2DDCF96F0438}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00F83E77-CFB6-41BF-902A-203086407F2E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1411A24-A325-490D-A0CD-A1910193027E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{02F4FD01-0C73-40F9-AD5F-74B5D3B2FC29}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <author>tc={290BB73A-EF1D-4E13-A19B-72DD54C9761C}</author>
   </authors>
   <commentList>
-    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{290BB73A-EF1D-4E13-A19B-72DD54C9761C}">
+    <comment ref="B14" authorId="0" shapeId="0" xr:uid="{290BB73A-EF1D-4E13-A19B-72DD54C9761C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
   <si>
     <t>Task Name</t>
   </si>
@@ -360,14 +360,50 @@
     <t>Read dataset into MySQL Workbench</t>
   </si>
   <si>
-    <t>Sandra</t>
+    <t>Next Section: Employee Satisfaction by Department - "Happiness Meter"</t>
+  </si>
+  <si>
+    <t>Develop the CSS: Colors, Background, Etc.</t>
+  </si>
+  <si>
+    <t>Add statistical correlation info below related to relationship between employee satisfaction by dept and employee job performance by dept.</t>
+  </si>
+  <si>
+    <t>Top of page in overview: Pie Chart on each category of the satisfaction rating for the whole dataset.</t>
+  </si>
+  <si>
+    <t>Top of page in overview: Box plot showing summary statistics of ages.</t>
+  </si>
+  <si>
+    <t>Placement</t>
+  </si>
+  <si>
+    <t>Fraol &amp; Alejandra</t>
+  </si>
+  <si>
+    <t>Funnel chart to show employee attrition?</t>
+  </si>
+  <si>
+    <t>Scatter Plot on what contributes to attrition - show attrition yes and attition no in the legend showing two different color codes. Build Y-axis to show Job Involvement X-axis years since last promotion.</t>
+  </si>
+  <si>
+    <t>Bar graph: Showing overall performance rating by department and broken down beside it by job role. Place department dropdown with this.</t>
+  </si>
+  <si>
+    <t>Line Graph on what contributes to salary hike - Performance Rating, Years in Current Role, Years with Current Manager - possibly use drop down showing education/education level.</t>
+  </si>
+  <si>
+    <t>Set up the Title Image Carasoul: "Recruit and Retain", About the Staff, Our Mission Statement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Move 4 images (summary stats) to show under the title slot: Total Employees, Age Box Plot, Average Performance Rating, Average Employee Satisfaction                                           </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,8 +449,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -454,6 +496,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -533,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -618,6 +666,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -636,16 +694,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,7 +1089,7 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="A14" dT="2021-02-02T22:44:04.67" personId="{980333BF-B200-4403-B1E3-1C6C58F93070}" id="{290BB73A-EF1D-4E13-A19B-72DD54C9761C}">
+  <threadedComment ref="B14" dT="2021-02-02T22:44:04.67" personId="{980333BF-B200-4403-B1E3-1C6C58F93070}" id="{290BB73A-EF1D-4E13-A19B-72DD54C9761C}">
     <text>The instructions for the step are available at https://zoom.us/rec/play/Qw04fYFMUsRIXLak1TvswfIDqmPwoV16FvN4WGobshjUTySXNjvFWznQNB5b5pZgs6qRZCUK2SbFpBXi.yUvOevLRk7398GsV ... 4:33 in the video</text>
   </threadedComment>
 </ThreadedComments>
@@ -1034,38 +1097,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401E91F5-96CF-4A59-947D-268E9EC6FF85}">
-  <dimension ref="A1:P27"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="69.7265625" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" customWidth="1"/>
-    <col min="4" max="4" width="28.1796875" style="44" customWidth="1"/>
-    <col min="5" max="5" width="32" style="44" customWidth="1"/>
+    <col min="1" max="1" width="19" style="1" customWidth="1"/>
+    <col min="2" max="2" width="69.7265625" customWidth="1"/>
+    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="4" max="4" width="26.54296875" customWidth="1"/>
+    <col min="5" max="5" width="28.1796875" style="38" customWidth="1"/>
+    <col min="6" max="6" width="32" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="30"/>
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
       <c r="I1" s="30"/>
@@ -1073,27 +1139,28 @@
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
-      <c r="N1" s="31"/>
+      <c r="N1" s="30"/>
       <c r="O1" s="31"/>
       <c r="P1" s="31"/>
-    </row>
-    <row r="2" spans="1:16" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="7" t="s">
+      <c r="Q1" s="31"/>
+    </row>
+    <row r="2" spans="1:17" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A2" s="49"/>
+      <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="C2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="28">
+      <c r="D2" s="28">
         <v>0</v>
-      </c>
-      <c r="D2" s="29">
-        <v>44228</v>
       </c>
       <c r="E2" s="29">
         <v>44228</v>
       </c>
-      <c r="F2" s="30"/>
+      <c r="F2" s="29">
+        <v>44228</v>
+      </c>
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
@@ -1101,28 +1168,29 @@
       <c r="K2" s="30"/>
       <c r="L2" s="30"/>
       <c r="M2" s="30"/>
-      <c r="N2" s="31"/>
+      <c r="N2" s="30"/>
       <c r="O2" s="31"/>
       <c r="P2" s="31"/>
-    </row>
-    <row r="3" spans="1:16" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A3" s="10" t="s">
+      <c r="Q2" s="31"/>
+    </row>
+    <row r="3" spans="1:17" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A3" s="49"/>
+      <c r="B3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="C3" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C3" s="28">
-        <f>E3-D3</f>
+      <c r="D3" s="28">
+        <f>F3-E3</f>
         <v>2</v>
       </c>
-      <c r="D3" s="29">
+      <c r="E3" s="29">
         <v>44229</v>
       </c>
-      <c r="E3" s="29">
+      <c r="F3" s="29">
         <v>44231</v>
       </c>
-      <c r="F3" s="30"/>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
@@ -1130,28 +1198,29 @@
       <c r="K3" s="30"/>
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
-      <c r="N3" s="31"/>
+      <c r="N3" s="30"/>
       <c r="O3" s="31"/>
       <c r="P3" s="31"/>
-    </row>
-    <row r="4" spans="1:16" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A4" s="10" t="s">
+      <c r="Q3" s="31"/>
+    </row>
+    <row r="4" spans="1:17" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A4" s="49"/>
+      <c r="B4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="C4" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="28">
-        <f>E4-D4</f>
+      <c r="D4" s="28">
+        <f>F4-E4</f>
         <v>2</v>
       </c>
-      <c r="D4" s="29">
+      <c r="E4" s="29">
         <v>44229</v>
       </c>
-      <c r="E4" s="29">
+      <c r="F4" s="29">
         <v>44231</v>
       </c>
-      <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
@@ -1159,22 +1228,23 @@
       <c r="K4" s="30"/>
       <c r="L4" s="30"/>
       <c r="M4" s="30"/>
-      <c r="N4" s="31"/>
+      <c r="N4" s="30"/>
       <c r="O4" s="31"/>
       <c r="P4" s="31"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="7" t="s">
+      <c r="Q4" s="31"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" s="49"/>
+      <c r="B5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="28">
-        <f t="shared" ref="C5:C12" si="0">E5-D5</f>
+      <c r="C5" s="27"/>
+      <c r="D5" s="28">
+        <f t="shared" ref="D5:D14" si="0">F5-E5</f>
         <v>0</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="31"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
       <c r="G5" s="31"/>
       <c r="H5" s="31"/>
       <c r="I5" s="31"/>
@@ -1185,25 +1255,26 @@
       <c r="N5" s="31"/>
       <c r="O5" s="31"/>
       <c r="P5" s="31"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="Q5" s="31"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" s="49"/>
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="28">
-        <f>E6-D6</f>
+      <c r="D6" s="28">
+        <f>F6-E6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="43">
+      <c r="E6" s="37">
         <v>44231</v>
       </c>
-      <c r="E6" s="43">
+      <c r="F6" s="37">
         <v>44231</v>
       </c>
-      <c r="F6" s="31"/>
       <c r="G6" s="31"/>
       <c r="H6" s="31"/>
       <c r="I6" s="31"/>
@@ -1214,25 +1285,26 @@
       <c r="N6" s="31"/>
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+      <c r="Q6" s="31"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" s="49"/>
+      <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="28">
+      <c r="D7" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D7" s="43">
+      <c r="E7" s="37">
         <v>44231</v>
       </c>
-      <c r="E7" s="43">
+      <c r="F7" s="37">
         <v>44231</v>
       </c>
-      <c r="F7" s="31"/>
       <c r="G7" s="31"/>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
@@ -1243,25 +1315,26 @@
       <c r="N7" s="31"/>
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="Q7" s="31"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" s="49"/>
+      <c r="B8" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="28">
+      <c r="D8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D8" s="43">
+      <c r="E8" s="37">
         <v>44231</v>
       </c>
-      <c r="E8" s="43">
+      <c r="F8" s="37">
         <v>44231</v>
       </c>
-      <c r="F8" s="31"/>
       <c r="G8" s="31"/>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
@@ -1272,25 +1345,25 @@
       <c r="N8" s="31"/>
       <c r="O8" s="31"/>
       <c r="P8" s="31"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+      <c r="Q8" s="31"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B9" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C9" s="28">
+      <c r="D9" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D9" s="43">
+      <c r="E9" s="37">
         <v>44231</v>
       </c>
-      <c r="E9" s="43">
+      <c r="F9" s="37">
         <v>44231</v>
       </c>
-      <c r="F9" s="31"/>
       <c r="G9" s="31"/>
       <c r="H9" s="31"/>
       <c r="I9" s="31"/>
@@ -1301,25 +1374,25 @@
       <c r="N9" s="31"/>
       <c r="O9" s="31"/>
       <c r="P9" s="31"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="Q9" s="31"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="28">
+      <c r="D10" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D10" s="43">
+      <c r="E10" s="37">
         <v>44231</v>
       </c>
-      <c r="E10" s="43">
+      <c r="F10" s="37">
         <v>44231</v>
       </c>
-      <c r="F10" s="31"/>
       <c r="G10" s="31"/>
       <c r="H10" s="31"/>
       <c r="I10" s="31"/>
@@ -1330,16 +1403,19 @@
       <c r="N10" s="31"/>
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A11" s="27" t="s">
+      <c r="Q10" s="31"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B11" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="43"/>
-      <c r="E11" s="43"/>
-      <c r="F11" s="31"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
@@ -1350,20 +1426,20 @@
       <c r="N11" s="31"/>
       <c r="O11" s="31"/>
       <c r="P11" s="31"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="Q11" s="31"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="43">
+      <c r="C12" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="28"/>
+      <c r="E12" s="37">
         <v>44231</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="F12" s="31"/>
+      <c r="F12" s="37"/>
       <c r="G12" s="31"/>
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
@@ -1374,12 +1450,19 @@
       <c r="N12" s="31"/>
       <c r="O12" s="31"/>
       <c r="P12" s="31"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+      <c r="Q12" s="31"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="31"/>
+      <c r="C13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="28"/>
+      <c r="E13" s="38">
+        <v>43866</v>
+      </c>
       <c r="G13" s="31"/>
       <c r="H13" s="31"/>
       <c r="I13" s="31"/>
@@ -1390,12 +1473,25 @@
       <c r="N13" s="31"/>
       <c r="O13" s="31"/>
       <c r="P13" s="31"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="Q13" s="31"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F14" s="31"/>
+      <c r="C14" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D14" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="38">
+        <v>43866</v>
+      </c>
+      <c r="F14" s="38">
+        <v>43866</v>
+      </c>
       <c r="G14" s="31"/>
       <c r="H14" s="31"/>
       <c r="I14" s="31"/>
@@ -1406,66 +1502,146 @@
       <c r="N14" s="31"/>
       <c r="O14" s="31"/>
       <c r="P14" s="31"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="Q14" s="31"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B15" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="C15" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="28"/>
+      <c r="E15" s="38">
+        <v>43866</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="46" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="28"/>
+    </row>
+    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="46" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>4</v>
+      </c>
+      <c r="B19" s="46" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="50" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="46" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="47" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B32" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" s="1" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{EB089E7F-51F4-45B7-A735-2EFD3C809893}">
-      <formula1>"Sandra, Alejandra, Sam, Fraol, Tsegaye, All, NA"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{EB089E7F-51F4-45B7-A735-2EFD3C809893}">
+      <formula1>"Sandra, Alejandra, Sam, Fraol, Fraol &amp; Alejandra, Tsegaye, All, NA"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1488,183 +1664,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36" t="s">
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36" t="s">
+      <c r="B3" s="40"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="39" t="s">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
-      <c r="H5" s="41"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="45"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="33" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
       <c r="G10" s="32" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
       <c r="G11" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
       <c r="G12" s="32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
       <c r="G13" s="32" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
       <c r="G14" s="32" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
       <c r="G15" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C16" s="36" t="s">
+      <c r="C16" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
       <c r="G16" s="32" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:D2"/>
@@ -1678,6 +1848,12 @@
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1746,126 +1922,126 @@
       <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="39" t="s">
         <v>79</v>
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="14"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="45" t="s">
+      <c r="A8" s="39" t="s">
         <v>80</v>
       </c>
       <c r="B8" s="18"/>
       <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="45" t="s">
+      <c r="A9" s="39" t="s">
         <v>81</v>
       </c>
       <c r="B9" s="18"/>
       <c r="C9" s="14"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="39" t="s">
         <v>82</v>
       </c>
       <c r="B10" s="18"/>
       <c r="C10" s="14"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="45" t="s">
+      <c r="A11" s="39" t="s">
         <v>83</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="14"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="39" t="s">
         <v>84</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="14"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="39" t="s">
         <v>85</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="14"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="45" t="s">
+      <c r="A14" s="39" t="s">
         <v>86</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="14"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="45" t="s">
+      <c r="A15" s="39" t="s">
         <v>87</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="14"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="39" t="s">
         <v>88</v>
       </c>
       <c r="B16" s="18"/>
       <c r="C16" s="14"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="45" t="s">
+      <c r="A17" s="39" t="s">
         <v>89</v>
       </c>
       <c r="B17" s="18"/>
       <c r="C17" s="14"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="39" t="s">
         <v>90</v>
       </c>
       <c r="B18" s="18"/>
       <c r="C18" s="14"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="45" t="s">
+      <c r="A19" s="39" t="s">
         <v>91</v>
       </c>
       <c r="B19" s="18"/>
       <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="45" t="s">
+      <c r="A20" s="39" t="s">
         <v>92</v>
       </c>
       <c r="B20" s="18"/>
       <c r="C20" s="14"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="45" t="s">
+      <c r="A21" s="39" t="s">
         <v>94</v>
       </c>
       <c r="B21" s="18"/>
       <c r="C21" s="14"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="45" t="s">
+      <c r="A22" s="39" t="s">
         <v>95</v>
       </c>
       <c r="B22" s="18"/>
       <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="39" t="s">
         <v>96</v>
       </c>
       <c r="B23" s="18"/>
       <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="39" t="s">
         <v>97</v>
       </c>
       <c r="B24" s="18"/>

</xml_diff>

<commit_message>
More Question Ideas in the Project Plan
</commit_message>
<xml_diff>
--- a/Project Plan/HR_Project_Schedule.xlsx
+++ b/Project Plan/HR_Project_Schedule.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SaNdE\HR_Analysis\Project Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1411A24-A325-490D-A0CD-A1910193027E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBDBFA8-D360-4A96-9D1A-89173C351BDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{02F4FD01-0C73-40F9-AD5F-74B5D3B2FC29}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="5" xr2:uid="{02F4FD01-0C73-40F9-AD5F-74B5D3B2FC29}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Schedule" sheetId="1" r:id="rId1"/>
     <sheet name="Team Roles" sheetId="2" r:id="rId2"/>
     <sheet name="Questions and Visualizations" sheetId="3" r:id="rId3"/>
     <sheet name="Project 3 Ideas" sheetId="4" r:id="rId4"/>
+    <sheet name="Phone Call Questions" sheetId="5" r:id="rId5"/>
+    <sheet name="New Ideas" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="126">
   <si>
     <t>Task Name</t>
   </si>
@@ -397,6 +399,42 @@
   </si>
   <si>
     <t xml:space="preserve">Move 4 images (summary stats) to show under the title slot: Total Employees, Age Box Plot, Average Performance Rating, Average Employee Satisfaction                                           </t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>What are the tools you find yourself using most often creating dashboards? What tools do you see used most among others in the field? Why?</t>
+  </si>
+  <si>
+    <t>Which metrics have you found company leaders to be most interested in learning about? Ie. Factors that contrbute to turn over? Factors that are highly correlated with top performers? Insights about salary distribution? Is training adding value--such as increasing job involvement, tenure, and satisfaction with the company? Turnover in the first year metrics?</t>
+  </si>
+  <si>
+    <t>Does job level directly correlate to salary level or are there outliers to evaluate?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What departments/job roles are working most of the overtime? </t>
+  </si>
+  <si>
+    <t>Visualize ages of employees in chunks of 50 with a histogram. See article.</t>
+  </si>
+  <si>
+    <t>Check for salary inequality by visualizing salary ranges by job level, role and, years of experience. Possibly also look at education.</t>
+  </si>
+  <si>
+    <t>Create an interactive logistical regression model to find which variables have highest significance against turnover and high performance.  Output into a user friendly format, not a statistical analysis on the front end.</t>
+  </si>
+  <si>
+    <t>Visualization Ideas for Data Story</t>
+  </si>
+  <si>
+    <t>Data Story</t>
+  </si>
+  <si>
+    <t>(A bit evil but…) Compare the highest salaries to the performance ratings. What a company spends the most money on, SHOULD BE giving them the greatest return. If it isn't, it might be time to create an action plan or "trim the fat", so to speak.</t>
   </si>
 </sst>
 </file>
@@ -581,7 +619,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -676,24 +714,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -707,6 +727,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1097,23 +1144,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401E91F5-96CF-4A59-947D-268E9EC6FF85}">
-  <dimension ref="A1:Q37"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="19" style="1" customWidth="1"/>
-    <col min="2" max="2" width="69.7265625" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
-    <col min="4" max="4" width="26.54296875" customWidth="1"/>
-    <col min="5" max="5" width="28.1796875" style="38" customWidth="1"/>
-    <col min="6" max="6" width="32" style="38" customWidth="1"/>
+    <col min="2" max="3" width="69.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" customWidth="1"/>
+    <col min="5" max="5" width="26.54296875" customWidth="1"/>
+    <col min="6" max="6" width="28.1796875" style="38" customWidth="1"/>
+    <col min="7" max="7" width="32" style="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.4">
       <c r="A1" s="11" t="s">
         <v>106</v>
       </c>
@@ -1121,18 +1168,20 @@
         <v>0</v>
       </c>
       <c r="C1" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="G1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="30"/>
       <c r="H1" s="30"/>
       <c r="I1" s="30"/>
       <c r="J1" s="30"/>
@@ -1140,28 +1189,29 @@
       <c r="L1" s="30"/>
       <c r="M1" s="30"/>
       <c r="N1" s="30"/>
-      <c r="O1" s="31"/>
+      <c r="O1" s="30"/>
       <c r="P1" s="31"/>
       <c r="Q1" s="31"/>
-    </row>
-    <row r="2" spans="1:17" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A2" s="49"/>
+      <c r="R1" s="31"/>
+    </row>
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A2" s="43"/>
       <c r="B2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="28">
+      <c r="E2" s="28">
         <v>0</v>
-      </c>
-      <c r="E2" s="29">
-        <v>44228</v>
       </c>
       <c r="F2" s="29">
         <v>44228</v>
       </c>
-      <c r="G2" s="30"/>
+      <c r="G2" s="29">
+        <v>44228</v>
+      </c>
       <c r="H2" s="30"/>
       <c r="I2" s="30"/>
       <c r="J2" s="30"/>
@@ -1169,29 +1219,30 @@
       <c r="L2" s="30"/>
       <c r="M2" s="30"/>
       <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
+      <c r="O2" s="30"/>
       <c r="P2" s="31"/>
       <c r="Q2" s="31"/>
-    </row>
-    <row r="3" spans="1:17" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A3" s="49"/>
+      <c r="R2" s="31"/>
+    </row>
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A3" s="43"/>
       <c r="B3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="10"/>
+      <c r="D3" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="28">
-        <f>F3-E3</f>
+      <c r="E3" s="28">
+        <f>G3-F3</f>
         <v>2</v>
       </c>
-      <c r="E3" s="29">
+      <c r="F3" s="29">
         <v>44229</v>
       </c>
-      <c r="F3" s="29">
+      <c r="G3" s="29">
         <v>44231</v>
       </c>
-      <c r="G3" s="30"/>
       <c r="H3" s="30"/>
       <c r="I3" s="30"/>
       <c r="J3" s="30"/>
@@ -1199,29 +1250,30 @@
       <c r="L3" s="30"/>
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
-      <c r="O3" s="31"/>
+      <c r="O3" s="30"/>
       <c r="P3" s="31"/>
       <c r="Q3" s="31"/>
-    </row>
-    <row r="4" spans="1:17" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
-      <c r="A4" s="49"/>
+      <c r="R3" s="31"/>
+    </row>
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="18" x14ac:dyDescent="0.4">
+      <c r="A4" s="43"/>
       <c r="B4" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="10"/>
+      <c r="D4" s="28" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="28">
-        <f>F4-E4</f>
+      <c r="E4" s="28">
+        <f>G4-F4</f>
         <v>2</v>
       </c>
-      <c r="E4" s="29">
+      <c r="F4" s="29">
         <v>44229</v>
       </c>
-      <c r="F4" s="29">
+      <c r="G4" s="29">
         <v>44231</v>
       </c>
-      <c r="G4" s="30"/>
       <c r="H4" s="30"/>
       <c r="I4" s="30"/>
       <c r="J4" s="30"/>
@@ -1229,23 +1281,24 @@
       <c r="L4" s="30"/>
       <c r="M4" s="30"/>
       <c r="N4" s="30"/>
-      <c r="O4" s="31"/>
+      <c r="O4" s="30"/>
       <c r="P4" s="31"/>
       <c r="Q4" s="31"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A5" s="49"/>
+      <c r="R4" s="31"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="43"/>
       <c r="B5" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28">
-        <f t="shared" ref="D5:D14" si="0">F5-E5</f>
+      <c r="C5" s="7"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="28">
+        <f t="shared" ref="E5:E14" si="0">G5-F5</f>
         <v>0</v>
       </c>
-      <c r="E5" s="36"/>
       <c r="F5" s="36"/>
-      <c r="G5" s="31"/>
+      <c r="G5" s="36"/>
       <c r="H5" s="31"/>
       <c r="I5" s="31"/>
       <c r="J5" s="31"/>
@@ -1256,26 +1309,27 @@
       <c r="O5" s="31"/>
       <c r="P5" s="31"/>
       <c r="Q5" s="31"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A6" s="49"/>
+      <c r="R5" s="31"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="43"/>
       <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="9"/>
+      <c r="D6" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="28">
-        <f>F6-E6</f>
+      <c r="E6" s="28">
+        <f>G6-F6</f>
         <v>0</v>
-      </c>
-      <c r="E6" s="37">
-        <v>44231</v>
       </c>
       <c r="F6" s="37">
         <v>44231</v>
       </c>
-      <c r="G6" s="31"/>
+      <c r="G6" s="37">
+        <v>44231</v>
+      </c>
       <c r="H6" s="31"/>
       <c r="I6" s="31"/>
       <c r="J6" s="31"/>
@@ -1286,26 +1340,27 @@
       <c r="O6" s="31"/>
       <c r="P6" s="31"/>
       <c r="Q6" s="31"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A7" s="49"/>
+      <c r="R6" s="31"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="43"/>
       <c r="B7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="28">
+      <c r="E7" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E7" s="37">
-        <v>44231</v>
-      </c>
       <c r="F7" s="37">
         <v>44231</v>
       </c>
-      <c r="G7" s="31"/>
+      <c r="G7" s="37">
+        <v>44231</v>
+      </c>
       <c r="H7" s="31"/>
       <c r="I7" s="31"/>
       <c r="J7" s="31"/>
@@ -1316,26 +1371,27 @@
       <c r="O7" s="31"/>
       <c r="P7" s="31"/>
       <c r="Q7" s="31"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
-      <c r="A8" s="49"/>
+      <c r="R7" s="31"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="43"/>
       <c r="B8" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D8" s="28">
+      <c r="E8" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E8" s="37">
-        <v>44231</v>
-      </c>
       <c r="F8" s="37">
         <v>44231</v>
       </c>
-      <c r="G8" s="31"/>
+      <c r="G8" s="37">
+        <v>44231</v>
+      </c>
       <c r="H8" s="31"/>
       <c r="I8" s="31"/>
       <c r="J8" s="31"/>
@@ -1346,25 +1402,26 @@
       <c r="O8" s="31"/>
       <c r="P8" s="31"/>
       <c r="Q8" s="31"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R8" s="31"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B9" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D9" s="28">
+      <c r="E9" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E9" s="37">
-        <v>44231</v>
-      </c>
       <c r="F9" s="37">
         <v>44231</v>
       </c>
-      <c r="G9" s="31"/>
+      <c r="G9" s="37">
+        <v>44231</v>
+      </c>
       <c r="H9" s="31"/>
       <c r="I9" s="31"/>
       <c r="J9" s="31"/>
@@ -1375,25 +1432,26 @@
       <c r="O9" s="31"/>
       <c r="P9" s="31"/>
       <c r="Q9" s="31"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R9" s="31"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="9"/>
+      <c r="D10" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="28">
+      <c r="E10" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E10" s="37">
-        <v>44231</v>
-      </c>
       <c r="F10" s="37">
         <v>44231</v>
       </c>
-      <c r="G10" s="31"/>
+      <c r="G10" s="37">
+        <v>44231</v>
+      </c>
       <c r="H10" s="31"/>
       <c r="I10" s="31"/>
       <c r="J10" s="31"/>
@@ -1404,19 +1462,20 @@
       <c r="O10" s="31"/>
       <c r="P10" s="31"/>
       <c r="Q10" s="31"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R10" s="31"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B11" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="28">
+      <c r="C11" s="27"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E11" s="37"/>
       <c r="F11" s="37"/>
-      <c r="G11" s="31"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="31"/>
       <c r="I11" s="31"/>
       <c r="J11" s="31"/>
@@ -1427,20 +1486,21 @@
       <c r="O11" s="31"/>
       <c r="P11" s="31"/>
       <c r="Q11" s="31"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R11" s="31"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="10"/>
+      <c r="D12" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="37">
+      <c r="E12" s="28"/>
+      <c r="F12" s="37">
         <v>44231</v>
       </c>
-      <c r="F12" s="37"/>
-      <c r="G12" s="31"/>
+      <c r="G12" s="37"/>
       <c r="H12" s="31"/>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
@@ -1451,19 +1511,20 @@
       <c r="O12" s="31"/>
       <c r="P12" s="31"/>
       <c r="Q12" s="31"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R12" s="31"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="38">
+      <c r="E13" s="28"/>
+      <c r="F13" s="38">
         <v>43866</v>
       </c>
-      <c r="G13" s="31"/>
       <c r="H13" s="31"/>
       <c r="I13" s="31"/>
       <c r="J13" s="31"/>
@@ -1474,25 +1535,26 @@
       <c r="O13" s="31"/>
       <c r="P13" s="31"/>
       <c r="Q13" s="31"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R13" s="31"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B14" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="28">
+      <c r="E14" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E14" s="38">
-        <v>43866</v>
-      </c>
       <c r="F14" s="38">
         <v>43866</v>
       </c>
-      <c r="G14" s="31"/>
+      <c r="G14" s="38">
+        <v>43866</v>
+      </c>
       <c r="H14" s="31"/>
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
@@ -1503,144 +1565,168 @@
       <c r="O14" s="31"/>
       <c r="P14" s="31"/>
       <c r="Q14" s="31"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R14" s="31"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="38">
+      <c r="E15" s="28"/>
+      <c r="F15" s="38">
         <v>43866</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>1</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="28"/>
-    </row>
-    <row r="17" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C16" s="40"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="28"/>
+    </row>
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>2</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="40" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17" s="40"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>4</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="40" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B20" s="50" t="s">
+      <c r="C19" s="40"/>
+    </row>
+    <row r="20" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B20" s="44" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B21" s="46" t="s">
+      <c r="C20" s="44"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B21" s="40" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="29" x14ac:dyDescent="0.35">
-      <c r="B22" s="46" t="s">
+      <c r="C21" s="40"/>
+    </row>
+    <row r="22" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="40" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B23" s="46" t="s">
+      <c r="C22" s="40"/>
+    </row>
+    <row r="23" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B23" s="40" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B24" s="48" t="s">
+      <c r="C23" s="40"/>
+    </row>
+    <row r="24" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="42" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24" s="42"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B25" s="3"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="B26" s="47" t="s">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B26" s="41" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26" s="41"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B28" s="2" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B29" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B30" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B32" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B33" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C37" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{EB089E7F-51F4-45B7-A735-2EFD3C809893}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{EB089E7F-51F4-45B7-A735-2EFD3C809893}">
       <formula1>"Sandra, Alejandra, Sam, Fraol, Fraol &amp; Alejandra, Tsegaye, All, NA"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1664,177 +1750,183 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40" t="s">
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40" t="s">
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="43" t="s">
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="45"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40" t="s">
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="40"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="45"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
       <c r="G9" s="33" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C10" s="40" t="s">
+      <c r="C10" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="32" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="32" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C12" s="40" t="s">
+      <c r="C12" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
       <c r="G12" s="32" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C13" s="40" t="s">
+      <c r="C13" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
+      <c r="D13" s="45"/>
+      <c r="E13" s="45"/>
+      <c r="F13" s="45"/>
       <c r="G13" s="32" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C14" s="40" t="s">
+      <c r="C14" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="45"/>
       <c r="G14" s="32" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="32" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
       <c r="G16" s="32" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="C15:F15"/>
     <mergeCell ref="C10:F10"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:D2"/>
@@ -1848,12 +1940,6 @@
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2264,4 +2350,100 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E391C812-F0DD-407A-BD2B-AA6CC3CFC937}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="52.08984375" customWidth="1"/>
+    <col min="2" max="2" width="78.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="51" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70C9599-65D2-43E9-84EF-B250E0C989E6}">
+  <dimension ref="A1:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="130.6328125" style="51" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="53" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="51" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="51" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="51" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>